<commit_message>
Updated code and input and output documents
The error I originally used was not the best to evaluate the model. I used the Root mean squared deviation to evaluate the model's predictions. I also added code to format the output of the Excel spreadsheet to look better.
</commit_message>
<xml_diff>
--- a/Movies Recomendations/Movies(Input).xlsx
+++ b/Movies Recomendations/Movies(Input).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminhogan/Library/Mobile Documents/com~apple~CloudDocs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminhogan/Documents/Python Coding Documents/Jupyter Notebook Document-Scripts-Files/Movies Recomendations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26A1617-5D5D-3D47-8950-A172CF825298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E27660E-4508-D74D-872C-51FF4C3D183D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="660" windowWidth="24360" windowHeight="15980" xr2:uid="{9844D88B-1FAC-744F-84F9-B295BD1B97C5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="58">
   <si>
     <t>Title</t>
   </si>
@@ -185,6 +185,30 @@
   </si>
   <si>
     <t>Avatar: The Way of Water</t>
+  </si>
+  <si>
+    <t>Rio</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>The Mario Moive</t>
+  </si>
+  <si>
+    <t>The Little Mermaid</t>
+  </si>
+  <si>
+    <t>Oppenheimer</t>
+  </si>
+  <si>
+    <t>Knock at the Cabin</t>
+  </si>
+  <si>
+    <t>Gaurdian's of the Galaxy pt. 3</t>
   </si>
 </sst>
 </file>
@@ -215,9 +239,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -227,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -238,19 +271,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -304,8 +331,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A9337C4C-741F-B24A-B0E8-2441C9BA4644}" name="Table1" displayName="Table1" ref="A1:G30" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G30" xr:uid="{A9337C4C-741F-B24A-B0E8-2441C9BA4644}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A9337C4C-741F-B24A-B0E8-2441C9BA4644}" name="Table1" displayName="Table1" ref="A1:G36" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G36" xr:uid="{A9337C4C-741F-B24A-B0E8-2441C9BA4644}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{8F5FB264-BA92-A34D-AE8F-225F8AF88647}" name="Title" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{3F8FF60A-6E09-BC45-9735-0CADE9996341}" name="Runtime " dataDxfId="5"/>
@@ -616,10 +643,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB28081-8ACF-374A-96B4-3E269EB92988}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -940,7 +968,7 @@
         <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="F14" s="1">
         <v>5</v>
@@ -1222,82 +1250,200 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="6">
+        <v>96</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="1">
+        <v>8</v>
+      </c>
+      <c r="G27" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B28" s="1">
         <v>112</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F28" s="1">
         <v>8</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G28" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B29" s="5">
         <v>107</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C29" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-    </row>
-    <row r="29" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+      <c r="E29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B30" s="5">
         <v>146</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="7" t="s">
+      <c r="C30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E30" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B31" s="5">
         <v>192</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="7" t="s">
+      <c r="C31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="6">
+        <v>105</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="6">
+        <v>100</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="6">
+        <v>150</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="6">
+        <v>110</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="6">
+        <v>120</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>